<commit_message>
changes made by rounding off to Billion
</commit_message>
<xml_diff>
--- a/Data/budget_information.xlsx
+++ b/Data/budget_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e322a5376987641a/Documents/PhD_Thesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{4B357C28-A6C5-4CAF-B682-9DC9EBA9DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66414CF4-B428-4CB5-86C2-FC9410940655}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{4B357C28-A6C5-4CAF-B682-9DC9EBA9DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{490AA9D7-FEA3-4E58-94D7-C52D52BC244A}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="19530" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="19530" windowHeight="11490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="2" r:id="rId1"/>
@@ -400,7 +400,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -426,6 +426,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -711,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -952,13 +953,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AC23"/>
+  <dimension ref="A1:AD23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,7 +981,7 @@
     <col min="25" max="29" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1999</v>
       </c>
@@ -1154,7 +1155,7 @@
         <v>6956471827.4499998</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2000</v>
       </c>
@@ -1234,8 +1235,12 @@
       <c r="AC3" s="10">
         <v>10724671970.859999</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD3" s="17">
+        <f>ROUND(AC3,9)/1000000000</f>
+        <v>10.724671970860001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2001</v>
       </c>
@@ -1316,7 +1321,7 @@
         <v>14410217083.989998</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2002</v>
       </c>
@@ -1397,7 +1402,7 @@
         <v>18227884448.560001</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2003</v>
       </c>
@@ -1479,7 +1484,7 @@
         <v>15102436942.389999</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2004</v>
       </c>
@@ -1562,7 +1567,7 @@
         <v>22770346235.389999</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2005</v>
       </c>
@@ -1645,7 +1650,7 @@
         <v>29601043040.630005</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2006</v>
       </c>
@@ -1728,7 +1733,7 @@
         <v>36797245472.529999</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2007</v>
       </c>
@@ -1811,7 +1816,7 @@
         <v>49905322571.32</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2008</v>
       </c>
@@ -1896,7 +1901,7 @@
         <v>64599358901.169998</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2009</v>
       </c>
@@ -1981,7 +1986,7 @@
         <v>59378307821.489998</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2010</v>
       </c>
@@ -2066,7 +2071,7 @@
         <v>70138060838.040009</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2011</v>
       </c>
@@ -2149,7 +2154,7 @@
         <v>71114496668.959991</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2012</v>
       </c>
@@ -2232,7 +2237,7 @@
         <v>95198308028.860001</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2013</v>
       </c>

</xml_diff>

<commit_message>
changes to the code
</commit_message>
<xml_diff>
--- a/Data/budget_information.xlsx
+++ b/Data/budget_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e322a5376987641a/Documents/PhD_Thesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{4B357C28-A6C5-4CAF-B682-9DC9EBA9DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{490AA9D7-FEA3-4E58-94D7-C52D52BC244A}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{4B357C28-A6C5-4CAF-B682-9DC9EBA9DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2641D07A-0463-4691-B971-CBE321D1D2D4}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="19530" windowHeight="11490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="2" r:id="rId1"/>
@@ -400,7 +400,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -426,7 +426,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -712,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -953,13 +952,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD23"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD4" sqref="AD4"/>
+      <selection pane="bottomRight" activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,7 +980,7 @@
     <col min="25" max="29" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1069,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1999</v>
       </c>
@@ -1155,7 +1154,7 @@
         <v>6956471827.4499998</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2000</v>
       </c>
@@ -1235,12 +1234,8 @@
       <c r="AC3" s="10">
         <v>10724671970.859999</v>
       </c>
-      <c r="AD3" s="17">
-        <f>ROUND(AC3,9)/1000000000</f>
-        <v>10.724671970860001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2001</v>
       </c>
@@ -1321,7 +1316,7 @@
         <v>14410217083.989998</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2002</v>
       </c>
@@ -1402,7 +1397,7 @@
         <v>18227884448.560001</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2003</v>
       </c>
@@ -1484,7 +1479,7 @@
         <v>15102436942.389999</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2004</v>
       </c>
@@ -1567,7 +1562,7 @@
         <v>22770346235.389999</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2005</v>
       </c>
@@ -1650,7 +1645,7 @@
         <v>29601043040.630005</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2006</v>
       </c>
@@ -1733,7 +1728,7 @@
         <v>36797245472.529999</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2007</v>
       </c>
@@ -1816,7 +1811,7 @@
         <v>49905322571.32</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2008</v>
       </c>
@@ -1901,7 +1896,7 @@
         <v>64599358901.169998</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2009</v>
       </c>
@@ -1986,7 +1981,7 @@
         <v>59378307821.489998</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2010</v>
       </c>
@@ -2071,7 +2066,7 @@
         <v>70138060838.040009</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2011</v>
       </c>
@@ -2154,7 +2149,7 @@
         <v>71114496668.959991</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2012</v>
       </c>
@@ -2237,7 +2232,7 @@
         <v>95198308028.860001</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2013</v>
       </c>

</xml_diff>